<commit_message>
PowerPoint likely complete, and I cleaned up some unnecessary files
</commit_message>
<xml_diff>
--- a/Documents/Completed Tasks.xlsx
+++ b/Documents/Completed Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>Task</t>
   </si>
@@ -100,6 +100,51 @@
   </si>
   <si>
     <t>Christian, Travis</t>
+  </si>
+  <si>
+    <t>Documents</t>
+  </si>
+  <si>
+    <t>Code Review Part I-III</t>
+  </si>
+  <si>
+    <t>Christian, Julie</t>
+  </si>
+  <si>
+    <t>Use Cases</t>
+  </si>
+  <si>
+    <t>Tests Skeleton</t>
+  </si>
+  <si>
+    <t>Gantt Chart</t>
+  </si>
+  <si>
+    <t>System Test Procedure</t>
+  </si>
+  <si>
+    <t>Regression Test Procedure</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Deployment Plan</t>
+  </si>
+  <si>
+    <t>Mid-Semester Presentation</t>
+  </si>
+  <si>
+    <t>This Presentation</t>
+  </si>
+  <si>
+    <t>Front End</t>
+  </si>
+  <si>
+    <t>Christian, Josh</t>
+  </si>
+  <si>
+    <t>Back End</t>
   </si>
 </sst>
 </file>
@@ -123,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,8 +193,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -273,11 +330,203 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -292,6 +541,63 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C20"/>
+  <dimension ref="B1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,158 +891,381 @@
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="21"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="22"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="E5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="E6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="22"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="E8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="E9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="E10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="E11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="22"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="E12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="22"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="E13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="E14" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="27"/>
+    </row>
+    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
+      <c r="E15" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
+      <c r="E16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="21"/>
+    </row>
+    <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="9"/>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="C17" s="9"/>
+      <c r="E17" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="F17" s="24"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="27"/>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="E18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="E19" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="21"/>
+    </row>
+    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="E20" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="24"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="27"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
+    <row r="23" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C23" s="8" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="38">
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E15:G15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>